<commit_message>
Updated BOM to reflect parts availability
</commit_message>
<xml_diff>
--- a/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
+++ b/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larsen\inspirefly\ContentCube_Battery_Board\battery_board_v2b\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E2F48523-8527-46E5-B4B4-53A9A30424C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0D63FE-0A6D-4624-B2E1-A57CB031AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18720" xr2:uid="{20A4ACF5-A417-4FCE-A251-FF7FC547556D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="233">
   <si>
     <t>Designation</t>
   </si>
@@ -514,9 +514,6 @@
     <t>R33</t>
   </si>
   <si>
-    <t>85k</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -716,6 +713,27 @@
   </si>
   <si>
     <t>AD8495ARMZ-R7CT-ND</t>
+  </si>
+  <si>
+    <t>490-5258-2-ND</t>
+  </si>
+  <si>
+    <t>732-3067-1-ND</t>
+  </si>
+  <si>
+    <t>732-3063-1-ND</t>
+  </si>
+  <si>
+    <t>296-25227-1-ND</t>
+  </si>
+  <si>
+    <t>YAG2159CT-ND</t>
+  </si>
+  <si>
+    <t>85.6k</t>
+  </si>
+  <si>
+    <t>2019-RN73R1JTTD8562F100TR-ND</t>
   </si>
 </sst>
 </file>
@@ -858,7 +876,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1038,12 +1056,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1205,14 +1217,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1646,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEEDC35-BA7B-40D4-8198-B0F92B870051}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1679,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" t="s">
         <v>211</v>
-      </c>
-      <c r="G1" t="s">
-        <v>212</v>
       </c>
       <c r="H1" t="s">
         <v>133</v>
@@ -1692,25 +1702,25 @@
       <c r="A2">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1718,25 +1728,25 @@
       <c r="A3">
         <v>31</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1744,25 +1754,25 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1770,25 +1780,25 @@
       <c r="A5">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="G5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1796,25 +1806,25 @@
       <c r="A6">
         <v>43</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>74</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1822,25 +1832,25 @@
       <c r="A7">
         <v>60</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>98</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="G7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1848,25 +1858,25 @@
       <c r="A8">
         <v>64</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>98</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1874,25 +1884,25 @@
       <c r="A9">
         <v>48</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>98</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="G9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1900,25 +1910,25 @@
       <c r="A10">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>98</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>130</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1926,25 +1936,25 @@
       <c r="A11">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>74</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1952,25 +1962,25 @@
       <c r="A12">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
         <v>7</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="G12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1978,25 +1988,25 @@
       <c r="A13">
         <v>71</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>102</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>103</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="G13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2004,51 +2014,51 @@
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="G14" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>3</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="F15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H15" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2056,25 +2066,25 @@
       <c r="A16">
         <v>73</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>94</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="G16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2082,25 +2092,25 @@
       <c r="A17">
         <v>65</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>200</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" t="s">
+        <v>212</v>
+      </c>
+      <c r="H17" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2108,25 +2118,25 @@
       <c r="A18">
         <v>70</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="G18" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2134,25 +2144,25 @@
       <c r="A19">
         <v>56</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="F19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" t="s">
+        <v>218</v>
+      </c>
+      <c r="H19" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2160,25 +2170,25 @@
       <c r="A20">
         <v>13</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>144</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>145</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="F20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" t="s">
+        <v>216</v>
+      </c>
+      <c r="H20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2186,25 +2196,25 @@
       <c r="A21">
         <v>37</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>168</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="F21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H21" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2212,25 +2222,25 @@
       <c r="A22">
         <v>34</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="F22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" t="s">
+        <v>216</v>
+      </c>
+      <c r="H22" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2238,25 +2248,25 @@
       <c r="A23">
         <v>72</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
         <v>207</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="F23" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" t="s">
+        <v>216</v>
+      </c>
+      <c r="H23" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2264,25 +2274,25 @@
       <c r="A24">
         <v>17</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>144</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>216</v>
+      </c>
+      <c r="H24" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2290,25 +2300,25 @@
       <c r="A25">
         <v>32</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2316,25 +2326,25 @@
       <c r="A26">
         <v>51</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" t="s">
+        <v>216</v>
+      </c>
+      <c r="H26" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2342,25 +2352,25 @@
       <c r="A27">
         <v>41</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>174</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="1" t="s">
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2368,25 +2378,25 @@
       <c r="A28">
         <v>18</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>151</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>144</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="F28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" t="s">
+        <v>216</v>
+      </c>
+      <c r="H28" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2394,25 +2404,25 @@
       <c r="A29">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
         <v>195</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="F29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" t="s">
+        <v>218</v>
+      </c>
+      <c r="H29" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2420,25 +2430,25 @@
       <c r="A30">
         <v>68</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>205</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H30" s="1" t="s">
+      <c r="F30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" t="s">
+        <v>218</v>
+      </c>
+      <c r="H30" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2446,25 +2456,25 @@
       <c r="A31">
         <v>15</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>146</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>147</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H31" s="1" t="s">
+      <c r="F31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" t="s">
+        <v>218</v>
+      </c>
+      <c r="H31" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2472,25 +2482,25 @@
       <c r="A32">
         <v>5</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>136</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H32" s="1" t="s">
+      <c r="F32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" t="s">
+        <v>219</v>
+      </c>
+      <c r="H32" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2498,25 +2508,25 @@
       <c r="A33">
         <v>26</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>144</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>157</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H33" s="1" t="s">
+      <c r="F33" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" t="s">
+        <v>216</v>
+      </c>
+      <c r="H33" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2524,25 +2534,25 @@
       <c r="A34">
         <v>54</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H34" s="1" t="s">
+      <c r="F34" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" t="s">
+        <v>216</v>
+      </c>
+      <c r="H34" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2550,25 +2560,25 @@
       <c r="A35">
         <v>57</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H35" s="1" t="s">
+      <c r="F35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" t="s">
+        <v>216</v>
+      </c>
+      <c r="H35" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2576,77 +2586,77 @@
       <c r="A36">
         <v>67</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
+        <v>201</v>
+      </c>
+      <c r="C36" t="s">
         <v>202</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
         <v>203</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H36" s="1" t="s">
+      <c r="F36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" t="s">
+        <v>217</v>
+      </c>
+      <c r="H36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>58</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="3">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A38" s="2">
+        <v>59</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A38" s="3">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" s="3">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="F38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H38" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2654,25 +2664,25 @@
       <c r="A39">
         <v>9</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H39" s="1" t="s">
+      <c r="G39" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2680,25 +2690,25 @@
       <c r="A40">
         <v>11</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>46</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H40" s="1" t="s">
+      <c r="G40" t="s">
+        <v>134</v>
+      </c>
+      <c r="H40" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2706,25 +2716,25 @@
       <c r="A41">
         <v>30</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
         <v>162</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
+        <v>223</v>
+      </c>
+      <c r="F41" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" t="s">
         <v>224</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2732,25 +2742,25 @@
       <c r="A42">
         <v>10</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>138</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>139</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>140</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H42" s="1" t="s">
+      <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
+        <v>213</v>
+      </c>
+      <c r="H42" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2758,25 +2768,25 @@
       <c r="A43">
         <v>49</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>86</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>84</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H43" s="1" t="s">
+      <c r="G43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2784,25 +2794,25 @@
       <c r="A44">
         <v>52</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" t="s">
         <v>179</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>180</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H44" s="1" t="s">
+      <c r="F44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44" t="s">
+        <v>214</v>
+      </c>
+      <c r="H44" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2810,25 +2820,25 @@
       <c r="A45">
         <v>50</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" t="s">
         <v>112</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H45" s="1" t="s">
+      <c r="G45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H45" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2836,25 +2846,25 @@
       <c r="A46">
         <v>2</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46">
         <v>3</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>78</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H46" s="1" t="s">
+      <c r="G46" t="s">
+        <v>134</v>
+      </c>
+      <c r="H46" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2862,25 +2872,25 @@
       <c r="A47">
         <v>20</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" t="s">
         <v>63</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H47" s="1" t="s">
+      <c r="G47" t="s">
+        <v>134</v>
+      </c>
+      <c r="H47" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2888,25 +2898,25 @@
       <c r="A48">
         <v>53</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>180</v>
+      <c r="B48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" t="s">
+        <v>179</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H48" s="1" t="s">
+      <c r="E48" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" t="s">
+        <v>134</v>
+      </c>
+      <c r="G48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H48" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2914,25 +2924,25 @@
       <c r="A49">
         <v>16</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>64</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" t="s">
         <v>66</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H49" s="1" t="s">
+      <c r="G49" t="s">
+        <v>134</v>
+      </c>
+      <c r="H49" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2940,51 +2950,51 @@
       <c r="A50">
         <v>36</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>81</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" t="s">
         <v>83</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H50" s="1" t="s">
+      <c r="G50" t="s">
+        <v>134</v>
+      </c>
+      <c r="H50" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A51" s="3">
+      <c r="A51" s="2">
         <v>28</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="3">
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H51" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2992,25 +3002,25 @@
       <c r="A52">
         <v>19</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>107</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" t="s">
         <v>109</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H52" s="1" t="s">
+      <c r="G52" t="s">
+        <v>134</v>
+      </c>
+      <c r="H52" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3018,51 +3028,51 @@
       <c r="A53">
         <v>74</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>104</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" t="s">
         <v>106</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H53" s="1" t="s">
+      <c r="G53" t="s">
+        <v>134</v>
+      </c>
+      <c r="H53" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A54" s="3">
+      <c r="A54" s="2">
         <v>63</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D54" s="3">
-        <v>1</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H54" s="1" t="s">
+      <c r="F54" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H54" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3070,25 +3080,25 @@
       <c r="A55">
         <v>46</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="E55" t="s">
+        <v>175</v>
+      </c>
+      <c r="F55" t="s">
         <v>68</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H55" s="1" t="s">
+      <c r="G55" t="s">
+        <v>134</v>
+      </c>
+      <c r="H55" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3096,25 +3106,25 @@
       <c r="A56">
         <v>7</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>70</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>69</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" t="s">
         <v>71</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H56" s="1" t="s">
+      <c r="G56" t="s">
+        <v>134</v>
+      </c>
+      <c r="H56" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3122,25 +3132,25 @@
       <c r="A57">
         <v>66</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57">
         <v>7</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>117</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" t="s">
         <v>119</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H57" s="1" t="s">
+      <c r="G57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H57" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3148,25 +3158,25 @@
       <c r="A58">
         <v>1</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58">
         <v>15</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" t="s">
         <v>128</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="1" t="s">
+      <c r="G58" t="s">
+        <v>134</v>
+      </c>
+      <c r="H58" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3174,25 +3184,25 @@
       <c r="A59">
         <v>24</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>10</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>123</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" t="s">
         <v>125</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H59" s="1" t="s">
+      <c r="G59" t="s">
+        <v>134</v>
+      </c>
+      <c r="H59" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3200,25 +3210,25 @@
       <c r="A60">
         <v>14</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>10</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>8</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H60" s="1" t="s">
+      <c r="G60" t="s">
+        <v>134</v>
+      </c>
+      <c r="H60" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3226,25 +3236,25 @@
       <c r="A61">
         <v>47</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>10</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>32</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" t="s">
         <v>34</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H61" s="1" t="s">
+      <c r="G61" t="s">
+        <v>134</v>
+      </c>
+      <c r="H61" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3252,25 +3262,25 @@
       <c r="A62">
         <v>45</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>4</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" t="s">
         <v>7</v>
       </c>
-      <c r="G62" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H62" s="1" t="s">
+      <c r="G62" t="s">
+        <v>134</v>
+      </c>
+      <c r="H62" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3278,25 +3288,25 @@
       <c r="A63">
         <v>39</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>39</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>38</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" t="s">
         <v>40</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H63" s="1" t="s">
+      <c r="G63" t="s">
+        <v>134</v>
+      </c>
+      <c r="H63" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3304,25 +3314,25 @@
       <c r="A64">
         <v>44</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>89</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>90</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>88</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" t="s">
         <v>91</v>
       </c>
-      <c r="G64" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H64" s="1" t="s">
+      <c r="G64" t="s">
+        <v>134</v>
+      </c>
+      <c r="H64" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3330,49 +3340,49 @@
       <c r="A65">
         <v>29</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
         <v>160</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H65" s="1" t="s">
+      <c r="F65" t="s">
+        <v>134</v>
+      </c>
+      <c r="G65" t="s">
+        <v>221</v>
+      </c>
+      <c r="H65" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A66" s="3">
+      <c r="A66" s="2">
         <v>69</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="3">
-        <v>1</v>
-      </c>
-      <c r="E66" s="4" t="s">
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H66" s="1" t="s">
+      <c r="F66" s="2"/>
+      <c r="G66" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H66" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3380,25 +3390,25 @@
       <c r="A67">
         <v>40</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" t="s">
         <v>170</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
         <v>171</v>
       </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H67" s="1" t="s">
+      <c r="F67" t="s">
+        <v>134</v>
+      </c>
+      <c r="G67" t="s">
+        <v>222</v>
+      </c>
+      <c r="H67" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3406,25 +3416,25 @@
       <c r="A68">
         <v>42</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>25</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>26</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" t="s">
         <v>27</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H68" s="1" t="s">
+      <c r="G68" t="s">
+        <v>134</v>
+      </c>
+      <c r="H68" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3432,25 +3442,25 @@
       <c r="A69">
         <v>38</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>120</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>120</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" t="s">
         <v>122</v>
       </c>
-      <c r="G69" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H69" s="1" t="s">
+      <c r="G69" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3458,25 +3468,25 @@
       <c r="A70">
         <v>55</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>36</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>14</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>35</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" t="s">
         <v>37</v>
       </c>
-      <c r="G70" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H70" s="1" t="s">
+      <c r="G70" t="s">
+        <v>134</v>
+      </c>
+      <c r="H70" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3484,25 +3494,25 @@
       <c r="A71">
         <v>75</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" t="s">
         <v>209</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H71" s="1" t="s">
+      <c r="E71" t="s">
+        <v>209</v>
+      </c>
+      <c r="F71" t="s">
+        <v>134</v>
+      </c>
+      <c r="G71" t="s">
+        <v>220</v>
+      </c>
+      <c r="H71" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3510,25 +3520,25 @@
       <c r="A72">
         <v>22</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>153</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>154</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>155</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H72" s="1" t="s">
+      <c r="F72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G72" t="s">
+        <v>225</v>
+      </c>
+      <c r="H72" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BOM for final parts order
</commit_message>
<xml_diff>
--- a/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
+++ b/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larse\OneDrive\Desktop\InspireFly\ContentCube_Battery_Board\battery_board_v2b\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86A6FD4-32F2-4FA0-9074-7D4ADBDFD267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CA896A-DE7D-449C-9DF4-9D412B54044A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{20A4ACF5-A417-4FCE-A251-FF7FC547556D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="233">
   <si>
     <t>Designation</t>
   </si>
@@ -716,6 +716,24 @@
   </si>
   <si>
     <t>AD8495ARMZ-R7CT-ND</t>
+  </si>
+  <si>
+    <t>296-25227-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	2019-RN73R1JTTD8562F100CT-ND</t>
+  </si>
+  <si>
+    <t>YAG2159CT-ND</t>
+  </si>
+  <si>
+    <t>732-3063-1-ND</t>
+  </si>
+  <si>
+    <t>732-3067-1-ND</t>
+  </si>
+  <si>
+    <t>490-5258-1-ND</t>
   </si>
 </sst>
 </file>
@@ -858,7 +876,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1038,12 +1056,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1210,7 +1222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1644,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEEDC35-BA7B-40D4-8198-B0F92B870051}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G15" sqref="A15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2044,7 +2056,7 @@
         <v>134</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>134</v>
+        <v>232</v>
       </c>
       <c r="H15" t="s">
         <v>134</v>
@@ -2616,7 +2628,7 @@
         <v>134</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>134</v>
+        <v>230</v>
       </c>
       <c r="H37" t="s">
         <v>134</v>
@@ -2642,7 +2654,7 @@
         <v>134</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="H38" t="s">
         <v>134</v>
@@ -2980,7 +2992,7 @@
         <v>134</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="H51" t="s">
         <v>134</v>
@@ -3058,7 +3070,7 @@
         <v>134</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>134</v>
+        <v>229</v>
       </c>
       <c r="H54" t="s">
         <v>134</v>
@@ -3368,7 +3380,7 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2" t="s">
-        <v>134</v>
+        <v>227</v>
       </c>
       <c r="H66" t="s">
         <v>134</v>
@@ -3532,8 +3544,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated 5v reg and lowside switch
</commit_message>
<xml_diff>
--- a/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
+++ b/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larse\OneDrive\Desktop\InspireFly\ContentCube_Battery_Board\battery_board_v2b\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CA896A-DE7D-449C-9DF4-9D412B54044A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E83AA41-3DC8-4E42-9EE1-DD298B00F129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{20A4ACF5-A417-4FCE-A251-FF7FC547556D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="BOM-battery_board_v1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">battery_board_v2b!$A$1:$H$72</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">battery_board_v2b!$A$1:$H$76</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="247">
   <si>
     <t>Designation</t>
   </si>
@@ -734,6 +734,48 @@
   </si>
   <si>
     <t>490-5258-1-ND</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>TPSM84209RKHT</t>
+  </si>
+  <si>
+    <t>C2836944</t>
+  </si>
+  <si>
+    <t>C16,C15,C18,C12,C13</t>
+  </si>
+  <si>
+    <t>R14,R40,R39,R50</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>330pF</t>
+  </si>
+  <si>
+    <t>C1664</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>C140782</t>
+  </si>
+  <si>
+    <t>C137777</t>
+  </si>
+  <si>
+    <t>1.37k</t>
+  </si>
+  <si>
+    <t>R45</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1318,10 +1360,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{425A8C04-4A4C-47E4-B366-38A044E8A39F}" name="battery_board_v2b" displayName="battery_board_v2b" ref="A1:H72" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H72" xr:uid="{425A8C04-4A4C-47E4-B366-38A044E8A39F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H72">
-    <sortCondition ref="B1:B72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{425A8C04-4A4C-47E4-B366-38A044E8A39F}" name="battery_board_v2b" displayName="battery_board_v2b" ref="A1:H76" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H76" xr:uid="{425A8C04-4A4C-47E4-B366-38A044E8A39F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H71">
+    <sortCondition ref="B1:B71"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B35D46FB-269C-49C8-A612-255C9F8E2975}" uniqueName="1" name="Id" queryTableFieldId="1"/>
@@ -1654,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEEDC35-BA7B-40D4-8198-B0F92B870051}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G15" sqref="A15:G15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1755,13 +1797,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>236</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>58</v>
@@ -1804,22 +1846,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="G6" t="s">
         <v>134</v>
@@ -1830,10 +1872,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
         <v>98</v>
@@ -1842,10 +1884,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
         <v>134</v>
@@ -1856,22 +1898,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>98</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="G8" t="s">
         <v>134</v>
@@ -1882,22 +1924,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
         <v>98</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="G9" t="s">
         <v>134</v>
@@ -1908,22 +1950,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
         <v>134</v>
@@ -1934,22 +1976,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
         <v>134</v>
@@ -1960,22 +2002,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
         <v>134</v>
@@ -1986,22 +2028,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
         <v>134</v>
@@ -2012,51 +2054,51 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" t="s">
         <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>134</v>
+        <v>232</v>
       </c>
       <c r="H14" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>232</v>
+      <c r="A15">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>134</v>
       </c>
       <c r="H15" t="s">
         <v>134</v>
@@ -2064,25 +2106,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>201</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="G16" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
       <c r="H16" t="s">
         <v>134</v>
@@ -2090,25 +2132,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>201</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>213</v>
+        <v>134</v>
       </c>
       <c r="H17" t="s">
         <v>134</v>
@@ -2116,25 +2158,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>186</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="H18" t="s">
         <v>134</v>
@@ -2142,25 +2184,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="F19" t="s">
         <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H19" t="s">
         <v>134</v>
@@ -2168,10 +2210,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
         <v>144</v>
@@ -2180,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="F20" t="s">
         <v>134</v>
@@ -2194,10 +2236,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
         <v>144</v>
@@ -2206,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F21" t="s">
         <v>134</v>
@@ -2220,10 +2262,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
         <v>144</v>
@@ -2232,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>167</v>
+        <v>208</v>
       </c>
       <c r="F22" t="s">
         <v>134</v>
@@ -2246,10 +2288,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="C23" t="s">
         <v>144</v>
@@ -2258,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
         <v>134</v>
@@ -2272,10 +2314,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="C24" t="s">
         <v>144</v>
@@ -2284,7 +2326,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="F24" t="s">
         <v>134</v>
@@ -2298,10 +2340,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="C25" t="s">
         <v>144</v>
@@ -2310,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="F25" t="s">
         <v>134</v>
@@ -2324,25 +2366,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F26" t="s">
         <v>134</v>
       </c>
       <c r="G26" t="s">
-        <v>217</v>
+        <v>134</v>
       </c>
       <c r="H26" t="s">
         <v>134</v>
@@ -2350,25 +2392,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
         <v>134</v>
       </c>
       <c r="G27" t="s">
-        <v>134</v>
+        <v>217</v>
       </c>
       <c r="H27" t="s">
         <v>134</v>
@@ -2376,25 +2418,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="F28" t="s">
         <v>134</v>
       </c>
       <c r="G28" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H28" t="s">
         <v>134</v>
@@ -2402,10 +2444,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C29" t="s">
         <v>147</v>
@@ -2414,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="F29" t="s">
         <v>134</v>
@@ -2428,10 +2470,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
         <v>147</v>
@@ -2440,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="F30" t="s">
         <v>134</v>
@@ -2454,25 +2496,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F31" t="s">
         <v>134</v>
       </c>
       <c r="G31" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H31" t="s">
         <v>134</v>
@@ -2480,25 +2522,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="F32" t="s">
         <v>134</v>
       </c>
       <c r="G32" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H32" t="s">
         <v>134</v>
@@ -2506,10 +2548,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
         <v>144</v>
@@ -2518,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="F33" t="s">
         <v>134</v>
@@ -2532,10 +2574,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C34" t="s">
         <v>144</v>
@@ -2544,7 +2586,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F34" t="s">
         <v>134</v>
@@ -2558,25 +2600,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="C35" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="F35" t="s">
         <v>134</v>
       </c>
       <c r="G35" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H35" t="s">
         <v>134</v>
@@ -2584,77 +2626,77 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C36" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="F36" t="s">
         <v>134</v>
       </c>
       <c r="G36" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="H36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="2">
-        <v>58</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="A37">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="2">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>230</v>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" t="s">
+        <v>231</v>
       </c>
       <c r="H37" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2">
-        <v>59</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>231</v>
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" t="s">
+        <v>134</v>
       </c>
       <c r="H38" t="s">
         <v>134</v>
@@ -2662,22 +2704,22 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="G39" t="s">
         <v>134</v>
@@ -2688,25 +2730,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>224</v>
       </c>
       <c r="F40" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="G40" t="s">
-        <v>134</v>
+        <v>225</v>
       </c>
       <c r="H40" t="s">
         <v>134</v>
@@ -2714,25 +2756,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>224</v>
+        <v>140</v>
       </c>
       <c r="F41" t="s">
         <v>134</v>
       </c>
       <c r="G41" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="H41" t="s">
         <v>134</v>
@@ -2740,25 +2782,25 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s">
-        <v>214</v>
+        <v>134</v>
       </c>
       <c r="H42" t="s">
         <v>134</v>
@@ -2766,25 +2808,25 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="G43" t="s">
-        <v>134</v>
+        <v>215</v>
       </c>
       <c r="H43" t="s">
         <v>134</v>
@@ -2792,25 +2834,25 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>179</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
       <c r="F44" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="G44" t="s">
-        <v>215</v>
+        <v>134</v>
       </c>
       <c r="H44" t="s">
         <v>134</v>
@@ -2818,22 +2860,22 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F45" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="G45" t="s">
         <v>134</v>
@@ -2844,22 +2886,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="G46" t="s">
         <v>134</v>
@@ -2870,25 +2912,25 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>61</v>
+        <v>183</v>
       </c>
       <c r="F47" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="G47" t="s">
-        <v>134</v>
+        <v>216</v>
       </c>
       <c r="H47" t="s">
         <v>134</v>
@@ -2896,25 +2938,25 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="G48" t="s">
-        <v>216</v>
+        <v>134</v>
       </c>
       <c r="H48" t="s">
         <v>134</v>
@@ -2922,10 +2964,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
@@ -2934,10 +2976,10 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="F49" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="G49" t="s">
         <v>134</v>
@@ -2948,10 +2990,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -2960,39 +3002,39 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="F50" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="G50" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="H50" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="2">
-        <v>28</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="A51">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="2">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>228</v>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" t="s">
+        <v>134</v>
       </c>
       <c r="H51" t="s">
         <v>134</v>
@@ -3000,22 +3042,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F52" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G52" t="s">
         <v>134</v>
@@ -3026,51 +3068,51 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>197</v>
       </c>
       <c r="C53" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>198</v>
+      </c>
+      <c r="F53" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" t="s">
+        <v>229</v>
+      </c>
+      <c r="H53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>46</v>
+      </c>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" t="s">
         <v>6</v>
       </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>104</v>
-      </c>
-      <c r="F53" t="s">
-        <v>106</v>
-      </c>
-      <c r="G53" t="s">
-        <v>134</v>
-      </c>
-      <c r="H53" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="2">
-        <v>63</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>229</v>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>176</v>
+      </c>
+      <c r="F54" t="s">
+        <v>68</v>
+      </c>
+      <c r="G54" t="s">
+        <v>134</v>
       </c>
       <c r="H54" t="s">
         <v>134</v>
@@ -3078,10 +3120,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -3090,10 +3132,10 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>176</v>
+        <v>69</v>
       </c>
       <c r="F55" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G55" t="s">
         <v>134</v>
@@ -3104,22 +3146,22 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="F56" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="G56" t="s">
         <v>134</v>
@@ -3130,22 +3172,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F57" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G57" t="s">
         <v>134</v>
@@ -3156,22 +3198,22 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D58">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F58" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G58" t="s">
         <v>134</v>
@@ -3182,22 +3224,22 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
         <v>10</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="G59" t="s">
         <v>134</v>
@@ -3208,22 +3250,22 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
         <v>10</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F60" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G60" t="s">
         <v>134</v>
@@ -3234,22 +3276,22 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G61" t="s">
         <v>134</v>
@@ -3260,22 +3302,22 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F62" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G62" t="s">
         <v>134</v>
@@ -3286,22 +3328,22 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="F63" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="G63" t="s">
         <v>134</v>
@@ -3312,25 +3354,25 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="F64" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="G64" t="s">
-        <v>134</v>
+        <v>222</v>
       </c>
       <c r="H64" t="s">
         <v>134</v>
@@ -3338,49 +3380,48 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
+        <v>69</v>
+      </c>
+      <c r="B65" t="s">
         <v>29</v>
       </c>
-      <c r="B65" t="s">
-        <v>160</v>
-      </c>
       <c r="C65" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
-      </c>
-      <c r="F65" t="s">
-        <v>134</v>
+        <v>28</v>
       </c>
       <c r="G65" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="H65" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="2">
-        <v>69</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2" t="s">
-        <v>227</v>
+      <c r="A66">
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" t="s">
+        <v>171</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66" t="s">
+        <v>134</v>
+      </c>
+      <c r="G66" t="s">
+        <v>223</v>
       </c>
       <c r="H66" t="s">
         <v>134</v>
@@ -3388,25 +3429,25 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="C67" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>172</v>
+        <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>134</v>
+        <v>27</v>
       </c>
       <c r="G67" t="s">
-        <v>223</v>
+        <v>134</v>
       </c>
       <c r="H67" t="s">
         <v>134</v>
@@ -3414,22 +3455,22 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>233</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>234</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>24</v>
+        <v>234</v>
       </c>
       <c r="F68" t="s">
-        <v>27</v>
+        <v>235</v>
       </c>
       <c r="G68" t="s">
         <v>134</v>
@@ -3440,22 +3481,22 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="F69" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="G69" t="s">
         <v>134</v>
@@ -3466,25 +3507,25 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>36</v>
+        <v>209</v>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>35</v>
+        <v>210</v>
       </c>
       <c r="F70" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="G70" t="s">
-        <v>134</v>
+        <v>221</v>
       </c>
       <c r="H70" t="s">
         <v>134</v>
@@ -3492,55 +3533,102 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B71" t="s">
-        <v>209</v>
+        <v>153</v>
       </c>
       <c r="C71" t="s">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>210</v>
+        <v>155</v>
       </c>
       <c r="F71" t="s">
         <v>134</v>
       </c>
       <c r="G71" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="H71" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72">
-        <v>22</v>
-      </c>
-      <c r="B72" t="s">
-        <v>153</v>
+      <c r="B72" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="C72" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
-      <c r="E72" t="s">
-        <v>155</v>
-      </c>
-      <c r="F72" t="s">
-        <v>134</v>
-      </c>
-      <c r="G72" t="s">
-        <v>226</v>
-      </c>
-      <c r="H72" t="s">
-        <v>134</v>
-      </c>
+      <c r="E72" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated files for manufacturing
</commit_message>
<xml_diff>
--- a/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
+++ b/battery_board_v2b/Manufacturing/BOM-battery_board_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larse\OneDrive\Desktop\InspireFly\ContentCube_Battery_Board\battery_board_v2b\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E83AA41-3DC8-4E42-9EE1-DD298B00F129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC6CD70-14D2-45E1-A0C1-4CAAA62F702A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{20A4ACF5-A417-4FCE-A251-FF7FC547556D}"/>
   </bookViews>
@@ -19,7 +19,20 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">battery_board_v2b!$A$1:$H$76</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="250">
   <si>
     <t>Designation</t>
   </si>
@@ -776,6 +789,15 @@
   </si>
   <si>
     <t>R45</t>
+  </si>
+  <si>
+    <t>C59461</t>
+  </si>
+  <si>
+    <t>C861548</t>
+  </si>
+  <si>
+    <t>C15525</t>
   </si>
 </sst>
 </file>
@@ -1259,12 +1281,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1696,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEEDC35-BA7B-40D4-8198-B0F92B870051}">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1757,7 +1778,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
@@ -1939,7 +1960,7 @@
         <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>130</v>
+        <v>249</v>
       </c>
       <c r="G9" t="s">
         <v>134</v>
@@ -3291,7 +3312,7 @@
         <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>7</v>
+        <v>248</v>
       </c>
       <c r="G61" t="s">
         <v>134</v>
@@ -3558,7 +3579,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B72" s="2" t="s">
+      <c r="B72" t="s">
         <v>238</v>
       </c>
       <c r="C72" t="s">
@@ -3567,17 +3588,15 @@
       <c r="D72">
         <v>1</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" t="s">
         <v>239</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" t="s">
         <v>240</v>
       </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B73" s="2" t="s">
+      <c r="B73" t="s">
         <v>241</v>
       </c>
       <c r="C73" t="s">
@@ -3586,49 +3605,29 @@
       <c r="D73">
         <v>1</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" t="s">
         <v>242</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" t="s">
         <v>243</v>
       </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B74" s="2" t="s">
+      <c r="B74" t="s">
         <v>246</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" t="s">
         <v>245</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" t="s">
         <v>244</v>
       </c>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>